<commit_message>
made edit to patients 2 data
</commit_message>
<xml_diff>
--- a/src/test_data/patients_2_specification.xlsx
+++ b/src/test_data/patients_2_specification.xlsx
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
-    <t>patients_1_specification.xlsx</t>
-  </si>
-  <si>
     <t>data_source</t>
   </si>
   <si>
@@ -82,13 +79,16 @@
   </si>
   <si>
     <t>Female</t>
+  </si>
+  <si>
+    <t>patients_2_specification.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -109,6 +109,22 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -127,8 +143,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -136,7 +154,9 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -469,7 +489,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -485,98 +505,98 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -616,6 +636,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>